<commit_message>
Math functions, if,ifs, count sum and average
</commit_message>
<xml_diff>
--- a/Formulas and Functions/2_Functions_Intro.xlsx
+++ b/Formulas and Functions/2_Functions_Intro.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lee\Desktop\Excel\Excel_Data_Analytics_Project\Formulas and Functions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF0403A4-62A4-4C02-BF36-3B20FBCE27C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90F189F6-7D05-44E2-AAC3-55169C010233}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{8CC555B5-3E06-43B6-9E5B-C0A1D3498DA4}"/>
   </bookViews>
@@ -980,8 +980,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8DE2224-2E95-4FCC-A032-AA541E0AE3D4}">
   <dimension ref="B1:S17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="P13" sqref="P13"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2505,7 +2505,7 @@
   <dimension ref="B2:D9"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>